<commit_message>
WorkDone 수정(최종 실패 시 Rethrow)
</commit_message>
<xml_diff>
--- a/Data/config.xlsx
+++ b/Data/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\Documents\UiPath\Template_CS\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B66EAE69-7336-41DB-8018-8EFF3856CD93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2710646-B972-42C6-8E5F-03610555400E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -423,7 +423,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>